<commit_message>
Comabt Narrative description - done + itemslist update
- comabt narrative description - done
- audio list - update
- particle effects list - update
</commit_message>
<xml_diff>
--- a/Game Design/Audio_Itemslist.xlsx
+++ b/Game Design/Audio_Itemslist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>#</t>
   </si>
@@ -163,6 +163,105 @@
   </si>
   <si>
     <t>opening sound track, sets the player in the mood for the game, slow start, builds up drama towards the end</t>
+  </si>
+  <si>
+    <t>A013</t>
+  </si>
+  <si>
+    <t>A014</t>
+  </si>
+  <si>
+    <t>A015</t>
+  </si>
+  <si>
+    <t>A016</t>
+  </si>
+  <si>
+    <t>A017</t>
+  </si>
+  <si>
+    <t>A018</t>
+  </si>
+  <si>
+    <t>A019</t>
+  </si>
+  <si>
+    <t>A020</t>
+  </si>
+  <si>
+    <t>Attack Shout (human)</t>
+  </si>
+  <si>
+    <t>units march (human)</t>
+  </si>
+  <si>
+    <t>Start Battle</t>
+  </si>
+  <si>
+    <t>world map to combat map, signals beginning of combat, battle drum sounding and slowly fading away in long echo while the view on your screen changes completely from the world map to the combat map in a blurry zoom like effect</t>
+  </si>
+  <si>
+    <t>Battle Music Track - Drama 1</t>
+  </si>
+  <si>
+    <t>Battle Music Track - Drama 2</t>
+  </si>
+  <si>
+    <t>Battle Music Track - Drama 3</t>
+  </si>
+  <si>
+    <t>the music in the combat mode, This music is more intense, faster, and wilder, a strong primeval beat from drums makes your shoulders shrink and your breathing fastens, it increases intensity and drama in multiple layers activated by the remaining hitpoint off all units in the battle, the less HPs remaining activate the next step in intensity and drama</t>
+  </si>
+  <si>
+    <t>sound of an arrow flying</t>
+  </si>
+  <si>
+    <t>sound of an arrow hitting</t>
+  </si>
+  <si>
+    <t>A021</t>
+  </si>
+  <si>
+    <t>A022</t>
+  </si>
+  <si>
+    <t>A023</t>
+  </si>
+  <si>
+    <t>A024</t>
+  </si>
+  <si>
+    <t>A025</t>
+  </si>
+  <si>
+    <t>A026</t>
+  </si>
+  <si>
+    <t>A027</t>
+  </si>
+  <si>
+    <t>A028</t>
+  </si>
+  <si>
+    <t>Horned Lion roar</t>
+  </si>
+  <si>
+    <t>Horned Lion roar lauder roar</t>
+  </si>
+  <si>
+    <t>unit hit by a claw attack</t>
+  </si>
+  <si>
+    <t>unit shout dying</t>
+  </si>
+  <si>
+    <t>End Battly Vicory</t>
+  </si>
+  <si>
+    <t>End Battly Defeat</t>
+  </si>
+  <si>
+    <t>a horn, cheerfull, epic, will give the player feeling of victory, domination, celebration, confidance, rewarding sound</t>
   </si>
 </sst>
 </file>
@@ -515,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +862,227 @@
       </c>
       <c r="G13" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
audio fix und main track
</commit_message>
<xml_diff>
--- a/Game Design/Audio_Itemslist.xlsx
+++ b/Game Design/Audio_Itemslist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -261,9 +261,6 @@
     <t>End Battly Vicory</t>
   </si>
   <si>
-    <t>End Battly Defeat</t>
-  </si>
-  <si>
     <t>a horn, cheerfull, epic, will give the player feeling of victory, domination, celebration, confidance, rewarding sound</t>
   </si>
   <si>
@@ -316,6 +313,21 @@
   </si>
   <si>
     <t>the player's unit armed with his axe hits an opponent</t>
+  </si>
+  <si>
+    <t>Blade Cuts Flesh</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Merrganaut hit</t>
+  </si>
+  <si>
+    <t>unit hit (Human)</t>
+  </si>
+  <si>
+    <t>End Battle Defeat</t>
   </si>
 </sst>
 </file>
@@ -670,7 +682,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -717,10 +731,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -737,13 +751,13 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
         <v>60</v>
@@ -780,7 +794,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
         <v>64</v>
@@ -797,10 +811,10 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -814,10 +828,10 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -834,7 +848,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,10 +865,10 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -862,19 +876,19 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
         <v>88</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -882,7 +896,7 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -891,33 +905,33 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="s">
         <v>97</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -934,7 +948,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s">
         <v>64</v>
@@ -954,7 +968,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>11</v>
@@ -977,7 +991,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -1000,7 +1014,7 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
         <v>25</v>
@@ -1020,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -1040,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
         <v>30</v>
@@ -1060,7 +1074,7 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
         <v>33</v>
@@ -1080,7 +1094,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -1100,7 +1114,7 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
         <v>44</v>
@@ -1120,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
         <v>45</v>
@@ -1140,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>47</v>
@@ -1163,7 +1177,7 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,7 +1194,7 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1197,7 +1211,7 @@
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,7 +1228,7 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -1234,7 +1248,7 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1242,7 +1256,7 @@
         <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -1251,10 +1265,10 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,7 +1285,7 @@
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G30" t="s">
         <v>64</v>
@@ -1279,17 +1293,44 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>96</v>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Battle sounds to Audio List
Various card attack sounds
Lion Death
Card selection sound
</commit_message>
<xml_diff>
--- a/Game Design/Audio_Itemslist.xlsx
+++ b/Game Design/Audio_Itemslist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -294,12 +294,39 @@
       <t>, a walking sound, steps (outdoor), (maybe) combined with heavy breathing</t>
     </r>
   </si>
+  <si>
+    <t>sliding rock tablet</t>
+  </si>
+  <si>
+    <t>each attack appears as a stone tablet, when you select it (or mouse over?) it slides up with a "sliding rocks" noise.</t>
+  </si>
+  <si>
+    <t>Horned Lion death</t>
+  </si>
+  <si>
+    <t>Healing Magic sound</t>
+  </si>
+  <si>
+    <t>Magic shield sound</t>
+  </si>
+  <si>
+    <t>A033</t>
+  </si>
+  <si>
+    <t>Lound swinging sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for powerful attacks </t>
+  </si>
+  <si>
+    <t>A034</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,7 +396,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="2" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,14 +405,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,9 +453,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,9 +487,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,9 +522,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -666,14 +698,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
@@ -681,7 +713,7 @@
     <col min="7" max="7" width="129.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -727,7 +759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -750,7 +782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -773,7 +805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -793,7 +825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -813,7 +845,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -833,7 +865,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -853,7 +885,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -873,7 +905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -893,7 +925,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -913,7 +945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -933,7 +965,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -953,7 +985,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -970,7 +1002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -987,7 +1019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1004,7 +1036,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1024,7 +1056,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1044,7 +1076,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -1064,7 +1096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1087,7 +1119,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -1107,19 +1139,95 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1137,24 +1245,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ressource Count Fix | FoW Fix
</commit_message>
<xml_diff>
--- a/Game Design/Audio_Itemslist.xlsx
+++ b/Game Design/Audio_Itemslist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
   <si>
     <t>#</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>DONE</t>
-  </si>
-  <si>
-    <t>check game play for reference</t>
   </si>
   <si>
     <t>Collect stone</t>
@@ -298,9 +295,6 @@
     <t>sliding rock tablet</t>
   </si>
   <si>
-    <t>each attack appears as a stone tablet, when you select it (or mouse over?) it slides up with a "sliding rocks" noise.</t>
-  </si>
-  <si>
     <t>Horned Lion death</t>
   </si>
   <si>
@@ -329,13 +323,98 @@
   </si>
   <si>
     <t>for when you aquire new powers (buy cards)</t>
+  </si>
+  <si>
+    <t>231537__vkproduktion__forest-birds-loop-02</t>
+  </si>
+  <si>
+    <t>Forest sound</t>
+  </si>
+  <si>
+    <t>A036</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>A037</t>
+  </si>
+  <si>
+    <t>76731__jobro__savanna-stomp-groove</t>
+  </si>
+  <si>
+    <t>Cool drum beat, maybe to use in menu or ingame</t>
+  </si>
+  <si>
+    <t>Tribal Drums</t>
+  </si>
+  <si>
+    <t>Jungle sound, maybe first 20 - 30 sec and then loop (?)</t>
+  </si>
+  <si>
+    <t>Jungle (Birds)</t>
+  </si>
+  <si>
+    <t>A038_2</t>
+  </si>
+  <si>
+    <t>A038_1</t>
+  </si>
+  <si>
+    <t>Jungle (insects)</t>
+  </si>
+  <si>
+    <t>184798__calcuttan__tropical-orchard-in-spring</t>
+  </si>
+  <si>
+    <t>177687__kyles__thailand-jungle-night-heavy-crickets1.flac</t>
+  </si>
+  <si>
+    <t>160756__cosmicembers__fast-swing-air-woosh</t>
+  </si>
+  <si>
+    <t>249818__spookymodem__magic-shield</t>
+  </si>
+  <si>
+    <t>From Toma: only the first 1 sec and then fade out (?)</t>
+  </si>
+  <si>
+    <t>106814__gunnbladez__120-concerta-male-choir-02</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DONE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>105280__mbezzola__stein-aufschlag-mit-langem-decay-03 oder 95000__j1987__cinderblockmove</t>
+  </si>
+  <si>
+    <t>(2 sfx in refference) each attack appears as a stone tablet, when you select it (or mouse over?) it slides up with a "sliding rocks" noise.</t>
+  </si>
+  <si>
+    <t>202145__junkfood2121__crunching</t>
+  </si>
+  <si>
+    <t>(first 3 sec) check game play for reference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +441,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,7 +492,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="2" builtinId="26"/>
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,9 +509,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -462,9 +549,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,7 +586,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,7 +621,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -708,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +918,7 @@
         <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -844,14 +931,17 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
+      <c r="D6" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
       </c>
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
       <c r="G6" s="4" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -859,19 +949,19 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E7" t="s">
         <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,19 +969,19 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
+      <c r="D8" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1153,19 +1243,22 @@
         <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
-        <v>6</v>
+      <c r="D22" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="E22" t="s">
         <v>52</v>
       </c>
+      <c r="F22" t="s">
+        <v>106</v>
+      </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,7 +1266,7 @@
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -1190,7 +1283,7 @@
         <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -1204,64 +1297,168 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
       </c>
-      <c r="D25" t="s">
-        <v>6</v>
+      <c r="D25" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E25" t="s">
         <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" t="s">
-        <v>6</v>
+      <c r="D26" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E26" t="s">
         <v>52</v>
       </c>
+      <c r="F26" t="s">
+        <v>101</v>
+      </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" t="s">
         <v>85</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" t="s">
         <v>86</v>
       </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">
-    <sortState ref="A2:G24">
+    <sortState ref="A2:G28">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>